<commit_message>
Update whole gas data with Philippine's updated QC column
</commit_message>
<xml_diff>
--- a/02_meter_data/gas_su_normalization.xlsx
+++ b/02_meter_data/gas_su_normalization.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734D87E2-CC34-4143-891C-E07C4FF8BB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5834A8-F012-9F49-97EC-31B03F4CD48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="500" windowWidth="15120" windowHeight="19540" activeTab="1" xr2:uid="{E854F3CC-68B1-C643-8758-04060BCC422B}"/>
+    <workbookView xWindow="5480" yWindow="1960" windowWidth="24360" windowHeight="19540" activeTab="1" xr2:uid="{E854F3CC-68B1-C643-8758-04060BCC422B}"/>
   </bookViews>
   <sheets>
     <sheet name="Standards" sheetId="1" r:id="rId1"/>
     <sheet name="Samples" sheetId="2" r:id="rId2"/>
     <sheet name="Normalization" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="167">
   <si>
     <t>Work Order</t>
   </si>
@@ -530,6 +530,15 @@
   </si>
   <si>
     <t>GC-11</t>
+  </si>
+  <si>
+    <t>Cannister A</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA </t>
   </si>
 </sst>
 </file>
@@ -1212,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DB90AC-603B-C54A-A166-8AF1848AABF6}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1783,7 +1792,7 @@
         <v>0.95600192347587021</v>
       </c>
     </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1794,7 +1803,7 @@
         <v>0.95171928088091129</v>
       </c>
     </row>
-    <row r="18" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K18" s="4" t="s">
         <v>31</v>
       </c>
@@ -1805,7 +1814,13 @@
         <v>0.94277008477388624</v>
       </c>
     </row>
-    <row r="19" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
       <c r="K19" s="4" t="s">
         <v>32</v>
       </c>
@@ -1816,7 +1831,16 @@
         <v>0.95519650780156762</v>
       </c>
     </row>
-    <row r="20" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.94</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.9</v>
+      </c>
       <c r="K20" s="4" t="s">
         <v>33</v>
       </c>
@@ -1827,7 +1851,16 @@
         <v>0.96869657032979273</v>
       </c>
     </row>
-    <row r="21" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>165</v>
+      </c>
       <c r="K21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1838,7 +1871,16 @@
         <v>0.94872609803186758</v>
       </c>
     </row>
-    <row r="22" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="4">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.9</v>
+      </c>
       <c r="K22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1849,7 +1891,16 @@
         <v>0.9481674767177477</v>
       </c>
     </row>
-    <row r="23" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="4">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>165</v>
+      </c>
       <c r="K23" s="4" t="s">
         <v>36</v>
       </c>
@@ -1860,7 +1911,16 @@
         <v>0.94807758308477907</v>
       </c>
     </row>
-    <row r="24" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="4">
+        <v>5</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.87</v>
+      </c>
       <c r="K24" s="4" t="s">
         <v>37</v>
       </c>
@@ -1871,7 +1931,16 @@
         <v>0.93513912792136544</v>
       </c>
     </row>
-    <row r="25" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="4">
+        <v>6</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.89</v>
+      </c>
       <c r="K25" s="4" t="s">
         <v>38</v>
       </c>
@@ -1880,6 +1949,94 @@
       </c>
       <c r="M25" s="3">
         <v>0.93513912792136544</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
+        <v>7</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="4">
+        <v>7</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.94</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="4">
+        <v>8</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="4">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="4">
+        <v>10</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" s="4">
+        <v>11</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="4">
+        <v>12</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="4">
+        <v>13</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>